<commit_message>
data down to 2018
</commit_message>
<xml_diff>
--- a/AAPL_financial_facts_with more fields.xlsx
+++ b/AAPL_financial_facts_with more fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albert/repo/jpmorgan/MLCOETSRL2026-question1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0A6714-E57C-CA4B-A0FD-B93176025C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC20008-E85A-544E-BDC9-9134290151D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1040" windowWidth="19620" windowHeight="25380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21340" yWindow="1040" windowWidth="19620" windowHeight="25380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0000320193_financial_facts" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9907" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9908" uniqueCount="169">
   <si>
     <t>Ticker</t>
   </si>
@@ -539,6 +539,9 @@
   </si>
   <si>
     <t>Depreciation (Reconciled Depreciation)</t>
+  </si>
+  <si>
+    <t>Inflation</t>
   </si>
 </sst>
 </file>
@@ -29833,7 +29836,7 @@
   <dimension ref="A1:N1445"/>
   <sheetViews>
     <sheetView topLeftCell="C821" zoomScale="111" workbookViewId="0">
-      <selection activeCell="F868" sqref="F868"/>
+      <selection activeCell="F868" sqref="A1:I1445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -71957,467 +71960,798 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25861809-6287-B14A-859C-E5C9A3D84DA8}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="76.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1">
+        <v>2017</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2018</v>
+      </c>
+      <c r="D1" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E1" s="6">
+        <v>2020</v>
+      </c>
+      <c r="F1" s="6">
         <v>2021</v>
       </c>
-      <c r="C1">
+      <c r="G1">
         <v>2022</v>
       </c>
-      <c r="D1">
+      <c r="H1">
         <v>2023</v>
       </c>
-      <c r="E1">
+      <c r="I1">
         <v>2024</v>
       </c>
-      <c r="F1">
+      <c r="J1">
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>365725000000</v>
+      </c>
+      <c r="D2">
+        <v>338516000000</v>
+      </c>
+      <c r="E2">
+        <v>323888000000</v>
+      </c>
+      <c r="F2">
+        <v>351002000000</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:I2" si="0">SUM(G3:G8)</f>
+        <v>352755000000</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>352583000000</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>364980000000</v>
+      </c>
+      <c r="J2">
+        <f>SUM(J3:J8)</f>
+        <v>359241000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>149</v>
       </c>
       <c r="C3">
+        <v>234386000000</v>
+      </c>
+      <c r="D3">
+        <v>175697000000</v>
+      </c>
+      <c r="E3">
+        <v>180175000000</v>
+      </c>
+      <c r="F3">
+        <v>216166000000</v>
+      </c>
+      <c r="G3">
         <v>217350000000</v>
       </c>
-      <c r="D3">
+      <c r="H3">
         <v>209017000000</v>
       </c>
-      <c r="E3">
+      <c r="I3">
         <v>211993000000</v>
       </c>
-      <c r="F3">
+      <c r="J3">
         <v>211284000000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>150</v>
       </c>
       <c r="C4">
+        <v>12087000000</v>
+      </c>
+      <c r="D4">
+        <v>12352000000</v>
+      </c>
+      <c r="E4">
+        <v>11264000000</v>
+      </c>
+      <c r="F4">
+        <v>14111000000</v>
+      </c>
+      <c r="G4">
         <v>21223000000</v>
       </c>
-      <c r="D4">
+      <c r="H4">
         <v>14695000000</v>
       </c>
-      <c r="E4">
+      <c r="I4">
         <v>14287000000</v>
       </c>
-      <c r="F4">
+      <c r="J4">
         <v>14585000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>151</v>
       </c>
       <c r="C5">
+        <f>C2-C3-C4-C6-C7-C8</f>
+        <v>48995000000</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:F5" si="1">D2-D3-D4-D6-D7-D8</f>
+        <v>45804000000</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>37445000000</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>51506000000</v>
+      </c>
+      <c r="G5">
         <v>60932000000</v>
       </c>
-      <c r="D5">
+      <c r="H5">
         <v>60985000000</v>
       </c>
-      <c r="E5">
+      <c r="I5">
         <v>66243000000</v>
       </c>
-      <c r="F5">
+      <c r="J5">
         <v>72957000000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>152</v>
       </c>
       <c r="B6">
+        <v>4855000000</v>
+      </c>
+      <c r="C6">
+        <v>3956000000</v>
+      </c>
+      <c r="D6">
+        <v>4106000000</v>
+      </c>
+      <c r="E6">
+        <v>4061000000</v>
+      </c>
+      <c r="F6">
         <v>6580000000</v>
       </c>
-      <c r="C6">
+      <c r="G6">
         <v>4946000000</v>
       </c>
-      <c r="D6">
+      <c r="H6">
         <v>6331000000</v>
       </c>
-      <c r="E6">
+      <c r="I6">
         <v>7286000000</v>
       </c>
-      <c r="F6">
+      <c r="J6">
         <v>5718000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>153</v>
       </c>
       <c r="C7">
+        <v>25913000000</v>
+      </c>
+      <c r="D7">
+        <v>48844000000</v>
+      </c>
+      <c r="E7">
+        <v>38016000000</v>
+      </c>
+      <c r="F7">
+        <v>34940000000</v>
+      </c>
+      <c r="G7">
         <v>23646000000</v>
       </c>
-      <c r="D7">
+      <c r="H7">
         <v>29965000000</v>
       </c>
-      <c r="E7">
+      <c r="I7">
         <v>29943000000</v>
       </c>
-      <c r="F7">
+      <c r="J7">
         <v>35934000000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>154</v>
       </c>
       <c r="C8">
+        <v>40388000000</v>
+      </c>
+      <c r="D8">
+        <v>51713000000</v>
+      </c>
+      <c r="E8">
+        <v>52927000000</v>
+      </c>
+      <c r="F8">
+        <v>27699000000</v>
+      </c>
+      <c r="G8">
         <v>24658000000</v>
       </c>
-      <c r="D8">
+      <c r="H8">
         <v>31590000000</v>
       </c>
-      <c r="E8">
+      <c r="I8">
         <v>35228000000</v>
       </c>
-      <c r="F8">
+      <c r="J8">
         <v>18763000000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>147</v>
       </c>
       <c r="C10">
+        <v>55888000000</v>
+      </c>
+      <c r="D10">
+        <v>46236000000</v>
+      </c>
+      <c r="E10">
+        <v>42296000000</v>
+      </c>
+      <c r="F10">
+        <v>54763000000</v>
+      </c>
+      <c r="G10">
         <v>64115000000</v>
       </c>
-      <c r="D10">
+      <c r="H10">
         <v>62611000000</v>
       </c>
-      <c r="E10">
+      <c r="I10">
         <v>68960000000</v>
       </c>
-      <c r="F10">
+      <c r="J10">
         <v>69860000000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>155</v>
       </c>
       <c r="C11">
+        <v>5966000000</v>
+      </c>
+      <c r="D11">
+        <v>5522000000</v>
+      </c>
+      <c r="E11">
+        <v>6643000000</v>
+      </c>
+      <c r="F11">
+        <v>7612000000</v>
+      </c>
+      <c r="G11">
         <v>7912000000</v>
       </c>
-      <c r="D11">
+      <c r="H11">
         <v>8061000000</v>
       </c>
-      <c r="E11">
+      <c r="I11">
         <v>8249000000</v>
       </c>
-      <c r="F11">
+      <c r="J11">
         <v>9055000000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>166</v>
       </c>
       <c r="C12">
+        <f t="shared" ref="C12:E12" si="2">C2-C15-C13-C11-C10</f>
+        <v>55012000000</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>53960000000</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>56453000000</v>
+      </c>
+      <c r="F12">
+        <f>F2-F15-F13-F11-F10</f>
+        <v>63106000000</v>
+      </c>
+      <c r="G12">
         <v>81955000000</v>
       </c>
-      <c r="D12">
+      <c r="H12">
         <v>74636000000</v>
       </c>
-      <c r="E12">
+      <c r="I12">
         <v>99183000000</v>
       </c>
-      <c r="F12">
+      <c r="J12">
         <v>86716000000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>156</v>
       </c>
       <c r="C13">
+        <v>141712000000</v>
+      </c>
+      <c r="D13">
+        <v>142310000000</v>
+      </c>
+      <c r="E13">
+        <v>153157000000</v>
+      </c>
+      <c r="F13">
+        <v>162431000000</v>
+      </c>
+      <c r="G13">
         <v>148101000000</v>
       </c>
-      <c r="D13">
+      <c r="H13">
         <v>145129000000</v>
       </c>
-      <c r="E13">
+      <c r="I13">
         <v>131638000000</v>
       </c>
-      <c r="F13">
+      <c r="J13">
         <v>119877000000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
       <c r="C15">
+        <v>107147000000</v>
+      </c>
+      <c r="D15">
+        <v>90488000000</v>
+      </c>
+      <c r="E15">
+        <v>65339000000</v>
+      </c>
+      <c r="F15">
+        <v>63090000000</v>
+      </c>
+      <c r="G15">
         <v>50672000000</v>
       </c>
-      <c r="D15">
+      <c r="H15">
         <v>62146000000</v>
       </c>
-      <c r="E15">
+      <c r="I15">
         <v>56950000000</v>
       </c>
-      <c r="F15">
+      <c r="J15">
         <v>73733000000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B16" s="4"/>
       <c r="C16">
-        <f t="shared" ref="C16" si="0">SUM(C3:C8) - SUM(C10:C13) - C15</f>
+        <f t="shared" ref="C16:F16" si="3">SUM(C3:C8) - SUM(C10:C13) - C15</f>
         <v>0</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16" si="1">SUM(D3:D8) - SUM(D10:D13) - D15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E16" si="2">SUM(E3:E8) - SUM(E10:E13) - E15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16" si="3">SUM(F3:F8) - SUM(F10:F13) - F15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <f>SUM(G3:G8) - SUM(G10:G13) - G15</f>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16" si="4">SUM(H3:H8) - SUM(H10:H13) - H15</f>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ref="I16" si="5">SUM(I3:I8) - SUM(I10:I13) - I15</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16" si="6">SUM(J3:J8) - SUM(J10:J13) - J15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>158</v>
       </c>
       <c r="C21">
+        <v>265595000000</v>
+      </c>
+      <c r="D21">
+        <v>260174000000</v>
+      </c>
+      <c r="E21">
+        <v>274515000000</v>
+      </c>
+      <c r="F21">
+        <v>365817000000</v>
+      </c>
+      <c r="G21">
         <v>394328000000</v>
       </c>
-      <c r="D21">
+      <c r="H21">
         <v>383285000000</v>
       </c>
-      <c r="E21">
+      <c r="I21">
         <v>391035000000</v>
       </c>
-      <c r="F21">
+      <c r="J21">
         <v>416161000000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>167</v>
       </c>
       <c r="C22">
+        <v>10903000000</v>
+      </c>
+      <c r="D22">
+        <v>12547000000</v>
+      </c>
+      <c r="E22">
+        <v>11056000000</v>
+      </c>
+      <c r="F22">
+        <v>11284000000</v>
+      </c>
+      <c r="G22">
+        <v>11104000000</v>
+      </c>
+      <c r="H22">
+        <v>11519000000</v>
+      </c>
+      <c r="I22">
+        <v>11445000000</v>
+      </c>
+      <c r="J22">
         <v>11698000000</v>
       </c>
-      <c r="D22">
-        <v>11445000000</v>
-      </c>
-      <c r="E22">
-        <v>11519000000</v>
-      </c>
-      <c r="F22">
-        <v>11104000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>159</v>
       </c>
       <c r="C23">
+        <v>152853000000</v>
+      </c>
+      <c r="D23">
+        <v>149235000000</v>
+      </c>
+      <c r="E23">
+        <v>158503000000</v>
+      </c>
+      <c r="F23">
+        <v>201697000000</v>
+      </c>
+      <c r="G23">
         <v>212442000000</v>
       </c>
-      <c r="D23">
+      <c r="H23">
         <v>202618000000</v>
       </c>
-      <c r="E23">
+      <c r="I23">
         <v>198907000000</v>
       </c>
-      <c r="F23">
+      <c r="J23">
         <v>209262000000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>160</v>
       </c>
       <c r="C24">
+        <v>30941000000</v>
+      </c>
+      <c r="D24">
+        <v>34462000000</v>
+      </c>
+      <c r="E24">
+        <v>38668000000</v>
+      </c>
+      <c r="F24">
+        <v>43887000000</v>
+      </c>
+      <c r="G24">
         <v>51345000000</v>
       </c>
-      <c r="D24">
+      <c r="H24">
         <v>54847000000</v>
       </c>
-      <c r="E24">
+      <c r="I24">
         <v>57467000000</v>
       </c>
-      <c r="F24">
+      <c r="J24">
         <v>62151000000</v>
       </c>
     </row>
-    <row r="25" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>161</v>
       </c>
       <c r="C25">
+        <v>13372000000</v>
+      </c>
+      <c r="D25">
+        <v>10481000000</v>
+      </c>
+      <c r="E25">
+        <v>9680000000</v>
+      </c>
+      <c r="F25">
+        <v>14527000000</v>
+      </c>
+      <c r="G25">
         <v>19300000000</v>
       </c>
-      <c r="D25">
+      <c r="H25">
         <v>16741000000</v>
       </c>
-      <c r="E25">
+      <c r="I25">
         <v>29749000000</v>
       </c>
-      <c r="F25">
+      <c r="J25">
         <v>20719000000</v>
       </c>
     </row>
-    <row r="26" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B26">
+      <c r="C26">
+        <v>59531000000</v>
+      </c>
+      <c r="D26">
+        <v>55256000000</v>
+      </c>
+      <c r="E26">
+        <v>57411000000</v>
+      </c>
+      <c r="F26">
         <v>94680000000</v>
       </c>
-      <c r="C26">
+      <c r="G26">
         <v>99803000000</v>
       </c>
-      <c r="D26">
+      <c r="H26">
         <v>96995000000</v>
       </c>
-      <c r="E26">
+      <c r="I26">
         <v>93736000000</v>
       </c>
-      <c r="F26">
+      <c r="J26">
         <v>112010000000</v>
       </c>
     </row>
-    <row r="31" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>163</v>
       </c>
       <c r="C32">
-        <v>-14841000000</v>
+        <v>13712000000</v>
       </c>
       <c r="D32">
-        <v>-15025000000</v>
+        <v>14119000000</v>
       </c>
       <c r="E32">
-        <v>-15234000000</v>
+        <v>14081000000</v>
       </c>
       <c r="F32">
-        <v>-15421000000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14467000000</v>
+      </c>
+      <c r="G32">
+        <v>14841000000</v>
+      </c>
+      <c r="H32">
+        <v>15025000000</v>
+      </c>
+      <c r="I32">
+        <v>15234000000</v>
+      </c>
+      <c r="J32">
+        <v>15421000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>164</v>
       </c>
       <c r="C33">
-        <v>-89402000000</v>
+        <v>72738000000</v>
       </c>
       <c r="D33">
-        <v>-77550000000</v>
+        <v>66897000000</v>
       </c>
       <c r="E33">
-        <v>-94949000000</v>
+        <v>72358000000</v>
       </c>
       <c r="F33">
-        <v>-90711000000</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B66" s="1"/>
+        <v>85971000000</v>
+      </c>
+      <c r="G33">
+        <v>89402000000</v>
+      </c>
+      <c r="H33">
+        <v>77550000000</v>
+      </c>
+      <c r="I33">
+        <v>94949000000</v>
+      </c>
+      <c r="J33">
+        <v>90711000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36">
+        <v>2.4E-2</v>
+      </c>
+      <c r="D36">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E36">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F36">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G36">
+        <v>0.08</v>
+      </c>
+      <c r="H36">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="I36">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="J36">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F66" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rough pdf extractor being implemented
</commit_message>
<xml_diff>
--- a/AAPL_financial_facts_with more fields.xlsx
+++ b/AAPL_financial_facts_with more fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albert/repo/jpmorgan/MLCOETSRL2026-question1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC20008-E85A-544E-BDC9-9134290151D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E72111-7E1F-9A4B-8766-84D4B3D934D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21340" yWindow="1040" windowWidth="19620" windowHeight="25380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9908" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9910" uniqueCount="171">
   <si>
     <t>Ticker</t>
   </si>
@@ -543,6 +543,12 @@
   <si>
     <t>Inflation</t>
   </si>
+  <si>
+    <t>total liquidity</t>
+  </si>
+  <si>
+    <t>cash as % of liquidity</t>
+  </si>
 </sst>
 </file>
 
@@ -1032,7 +1038,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1041,7 +1047,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1492,6 +1497,380 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Total</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Liabilities</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Liabilities!$AL$32:$AL$45</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>43373</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43737</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43737</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44465</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44465</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44829</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44829</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45564</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45564</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Liabilities!$AM$32:$AM$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>258578000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>248028000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>248028000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>258549000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>258549000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>287912000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>287912000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>302083000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>302083000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>290437000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>290437000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>308030000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>308030000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>285508000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6AC7-D94A-B333-E6AB273B4F70}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2091627376"/>
+        <c:axId val="1959875535"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="2091627376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1959875535"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1959875535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2091627376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Accounts payable current</a:t>
             </a:r>
           </a:p>
@@ -1826,7 +2205,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2159,7 +2538,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2492,7 +2871,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2833,7 +3212,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3174,7 +3553,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3632,7 +4011,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3965,7 +4344,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4310,7 +4689,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4588,339 +4967,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2051518287"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Other assets, current</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Assets!$D$77:$D$84</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>43373</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43737</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44101</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44465</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44829</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45200</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45564</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45928</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Assets!$E$77:$E$84</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>12087000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12352000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11264000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14111000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21223000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14695000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14287000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14585000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5B61-4645-B67F-A391FB94FED4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1795819311"/>
-        <c:axId val="1795631183"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="1795819311"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1795631183"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="months"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="1795631183"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1795819311"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5416,6 +5462,339 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Other assets, current</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Assets!$D$77:$D$84</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>43373</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43737</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44465</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44829</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45564</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Assets!$E$77:$E$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>12087000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12352000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11264000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14111000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21223000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14695000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14287000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14585000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B61-4645-B67F-A391FB94FED4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1795819311"/>
+        <c:axId val="1795631183"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1795819311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1795631183"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1795631183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1795819311"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Other assets, non-current</a:t>
             </a:r>
           </a:p>
@@ -5714,7 +6093,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6055,7 +6434,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6388,7 +6767,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6721,7 +7100,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7054,7 +7433,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7387,7 +7766,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7725,7 +8104,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -8058,7 +8437,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -8391,7 +8770,314 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>cash as % of liquidity</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Needed!$C$44:$J$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.39083875054674894</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48573445906301899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.41802007851071549</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55779945401427222</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48952467704537928</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48680042238648363</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45945282410888277</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65696473298352742</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4A8D-A34F-9116-B67FBF068052}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1084335424"/>
+        <c:axId val="1084337184"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1084335424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1084337184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1084337184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1084335424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -8724,340 +9410,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Cash equivalent</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Assets!$Y$35:$Y$42</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>43373</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43737</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44101</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44465</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44829</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45200</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45564</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45928</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Assets!$Z$35:$Z$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>25913000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>48844000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>38016000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34940000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>23646000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29965000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29943000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35934000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D35A-DB44-BDCF-9F938E680771}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="2051518287"/>
-        <c:axId val="2051634351"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="2051518287"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2051634351"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="months"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="2051634351"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2051518287"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -9425,6 +9778,339 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Cash equivalent</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Assets!$Y$35:$Y$42</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>43373</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43737</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44465</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44829</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45564</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Assets!$Z$35:$Z$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25913000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48844000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38016000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34940000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23646000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29965000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29943000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35934000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D35A-DB44-BDCF-9F938E680771}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2051518287"/>
+        <c:axId val="2051634351"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="2051518287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2051634351"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="2051634351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2051518287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Total sales</a:t>
             </a:r>
           </a:p>
@@ -9723,7 +10409,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -10056,7 +10742,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -10509,7 +11195,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -10967,7 +11653,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -11310,380 +11996,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1182671232"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Total</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Liabilities</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Liabilities!$AL$32:$AL$45</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>43373</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43737</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43737</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44101</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44101</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44465</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44465</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44829</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45200</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>45200</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>45564</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>45564</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>45928</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Liabilities!$AM$32:$AM$45</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>258578000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>248028000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>248028000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>258549000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>258549000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>287912000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>287912000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>302083000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>302083000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>290437000000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>290437000000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>308030000000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>308030000000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>285508000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6AC7-D94A-B333-E6AB273B4F70}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="2091627376"/>
-        <c:axId val="1959875535"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="2091627376"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1959875535"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="1959875535"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2091627376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12699,6 +13011,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors31.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -25323,6 +25675,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style31.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -28497,6 +29365,47 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ED55920-E992-D68E-98E0-EA13ED4FAE41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -28613,7 +29522,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -29022,7 +29931,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -29063,7 +29972,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -71962,8 +72871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25861809-6287-B14A-859C-E5C9A3D84DA8}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:J36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -71983,16 +72892,16 @@
       <c r="B1">
         <v>2017</v>
       </c>
-      <c r="C1" s="6">
+      <c r="C1">
         <v>2018</v>
       </c>
-      <c r="D1" s="6">
+      <c r="D1">
         <v>2019</v>
       </c>
-      <c r="E1" s="6">
+      <c r="E1">
         <v>2020</v>
       </c>
-      <c r="F1" s="6">
+      <c r="F1">
         <v>2021</v>
       </c>
       <c r="G1">
@@ -72705,6 +73614,80 @@
         <v>2.7E-2</v>
       </c>
     </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C43">
+        <f>SUM(C7:C8)</f>
+        <v>66301000000</v>
+      </c>
+      <c r="D43">
+        <f>SUM(D7:D8)</f>
+        <v>100557000000</v>
+      </c>
+      <c r="E43">
+        <f>SUM(E7:E8)</f>
+        <v>90943000000</v>
+      </c>
+      <c r="F43">
+        <f>SUM(F7:F8)</f>
+        <v>62639000000</v>
+      </c>
+      <c r="G43">
+        <f>SUM(G7:G8)</f>
+        <v>48304000000</v>
+      </c>
+      <c r="H43">
+        <f>SUM(H7:H8)</f>
+        <v>61555000000</v>
+      </c>
+      <c r="I43">
+        <f>SUM(I7:I8)</f>
+        <v>65171000000</v>
+      </c>
+      <c r="J43">
+        <f>SUM(J7:J8)</f>
+        <v>54697000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44">
+        <f>C7/C43</f>
+        <v>0.39083875054674894</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ref="D44:J44" si="7">D7/D43</f>
+        <v>0.48573445906301899</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="7"/>
+        <v>0.41802007851071549</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="7"/>
+        <v>0.55779945401427222</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="7"/>
+        <v>0.48952467704537928</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="7"/>
+        <v>0.48680042238648363</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="7"/>
+        <v>0.45945282410888277</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="7"/>
+        <v>0.65696473298352742</v>
+      </c>
+    </row>
     <row r="51" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F51" s="1"/>
     </row>
@@ -72755,6 +73738,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>